<commit_message>
Updating data .npz files just in case angles are still off (possibly for gesture 5)
</commit_message>
<xml_diff>
--- a/data/GPR_results.xlsx
+++ b/data/GPR_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmoln\Documents\Projects\NonAnthroHands_User_Study\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{879487FC-E957-462D-AAFB-C1C5CDA9D8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535DD7F8-622A-4953-B2C9-BFF2FC4847D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BD5C1CDC-D0A4-4C39-BDBC-142E97855F05}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Gesture #</t>
   </si>
@@ -72,14 +72,23 @@
     </r>
   </si>
   <si>
-    <t>Video</t>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Alpha value = 0.01, tuned on gesture 0</t>
+  </si>
+  <si>
+    <t>Is gesture 8 a subset of the other gestures? What makes it so low?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +122,23 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -140,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -193,11 +219,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF800080"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF800080"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF800080"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF800080"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -220,7 +393,50 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -229,6 +445,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF800080"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -253,7 +474,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>98461</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>65715</xdr:rowOff>
+      <xdr:rowOff>65716</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -586,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEB89D3-1F71-459C-9198-81CBF411CCF4}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,10 +823,12 @@
     <col min="6" max="6" width="15.109375" customWidth="1"/>
     <col min="7" max="7" width="18.109375" customWidth="1"/>
     <col min="8" max="9" width="19.21875" customWidth="1"/>
-    <col min="10" max="10" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" style="22" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" style="22" customWidth="1"/>
+    <col min="12" max="12" width="32.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,11 +856,17 @@
       <c r="I1" s="1">
         <v>7</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="16">
         <v>8</v>
       </c>
+      <c r="K1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="81.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="81.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -649,9 +878,11 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:10" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -663,88 +894,88 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+    <row r="4" spans="1:12" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="C4" s="6">
+        <v>6.8890000000000002</v>
+      </c>
+      <c r="D4" s="6">
+        <v>9.657</v>
+      </c>
+      <c r="E4" s="6">
+        <v>7.8680000000000003</v>
+      </c>
+      <c r="F4" s="6">
+        <v>10.789</v>
+      </c>
+      <c r="G4" s="6">
+        <v>7.0910000000000002</v>
+      </c>
+      <c r="H4" s="6">
+        <v>9.5749999999999993</v>
+      </c>
+      <c r="I4" s="6">
+        <v>8.7230000000000008</v>
+      </c>
+      <c r="J4" s="19">
+        <v>7.34</v>
+      </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="11" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7">
-        <v>0.81399999999999995</v>
-      </c>
-      <c r="C5" s="6">
-        <v>6.8890000000000002</v>
-      </c>
-      <c r="D5" s="6">
-        <v>9.657</v>
-      </c>
-      <c r="E5" s="6">
-        <v>7.8680000000000003</v>
-      </c>
-      <c r="F5" s="6">
-        <v>10.789</v>
-      </c>
-      <c r="G5" s="6">
-        <v>7.0910000000000002</v>
-      </c>
-      <c r="H5" s="6">
-        <v>9.5749999999999993</v>
-      </c>
-      <c r="I5" s="6">
-        <v>8.7230000000000008</v>
-      </c>
-      <c r="J5" s="6">
-        <v>7.34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="102" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+    <row r="5" spans="1:12" ht="102" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B5" s="4">
         <v>7.7149999999999999</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C5" s="4">
         <v>5.665</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D5" s="4">
         <v>6.4320000000000004</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E5" s="4">
         <v>7.9189999999999996</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F5" s="4">
         <v>5.3789999999999996</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G5" s="4">
         <v>11.05</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H5" s="4">
         <v>12.901</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I5" s="4">
         <v>7.0209999999999999</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J5" s="20">
         <v>0.316</v>
+      </c>
+      <c r="K5" s="21">
+        <f>ROUND( AVERAGE(B5:J5),3)</f>
+        <v>7.1550000000000002</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating record of errors and best alphas
</commit_message>
<xml_diff>
--- a/data/GPR_results.xlsx
+++ b/data/GPR_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmoln\Documents\Projects\NonAnthroHands_User_Study\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535DD7F8-622A-4953-B2C9-BFF2FC4847D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3171446B-994A-456F-B46F-9D135627DB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BD5C1CDC-D0A4-4C39-BDBC-142E97855F05}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Gesture #</t>
   </si>
@@ -83,12 +83,49 @@
   <si>
     <t>Is gesture 8 a subset of the other gestures? What makes it so low?</t>
   </si>
+  <si>
+    <t>Alpha = 1e-5</t>
+  </si>
+  <si>
+    <t>Leave-one-run-out, cross-validation error (why is it different than the above? Mislabeling between stored and retrieved error files?)</t>
+  </si>
+  <si>
+    <t>This isn’t correct K-fold cross-validation: I summed only the means (not MSE) for each run, and then neglected to divide by K</t>
+  </si>
+  <si>
+    <t>(Above data was strictly the mean value per run, summed across all runs. Not proper k-fold validation. Updating to reflect sum of MSEs per run, divided by the 10 runs:)</t>
+  </si>
+  <si>
+    <t>&lt;--Best overall choice</t>
+  </si>
+  <si>
+    <t>^ difficult to fit</t>
+  </si>
+  <si>
+    <t>^ easy to fit</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Error within gesture </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>(leave-one-run-out error, cross-validated), optimum alpha per run</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Prediction of unseen trajectory </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,8 +176,34 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +228,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3BAB5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -370,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -393,10 +462,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -438,6 +507,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="10" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEB89D3-1F71-459C-9198-81CBF411CCF4}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="54" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,7 +986,7 @@
       <c r="K1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -880,7 +1004,9 @@
       <c r="I2" s="3"/>
       <c r="J2" s="17"/>
       <c r="K2" s="13"/>
-      <c r="L2" s="9"/>
+      <c r="L2" s="30" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -973,6 +1099,714 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24">
+        <v>1.43</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.76</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.54</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.54</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I10" s="24">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="J10" s="24">
+        <v>0.83599999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="25">
+        <v>1E-4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.57</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.68</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="J11" s="26">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="27">
+        <v>1E-3</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.55</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.183</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1.32</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1.32</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0.501</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.58899999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1.05</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1.03</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.878</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2.13</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.34</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.251</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.85099999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="28">
+        <v>1</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1.28</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.503</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="27">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1.97</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.23</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1.69</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1.56</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1.93</v>
+      </c>
+      <c r="J16" s="4">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="28">
+        <v>100</v>
+      </c>
+      <c r="B17" s="6">
+        <v>3.41</v>
+      </c>
+      <c r="C17" s="6">
+        <v>4.24</v>
+      </c>
+      <c r="D17" s="6">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="E17" s="6">
+        <v>2.59</v>
+      </c>
+      <c r="F17" s="6">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="G17" s="7">
+        <v>1.81</v>
+      </c>
+      <c r="H17" s="6">
+        <v>3.66</v>
+      </c>
+      <c r="I17" s="6">
+        <v>4.13</v>
+      </c>
+      <c r="J17" s="6">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="35">
+        <v>0</v>
+      </c>
+      <c r="C20" s="35">
+        <v>1</v>
+      </c>
+      <c r="D20" s="35">
+        <v>2</v>
+      </c>
+      <c r="E20" s="35">
+        <v>3</v>
+      </c>
+      <c r="F20" s="35">
+        <v>4</v>
+      </c>
+      <c r="G20" s="35">
+        <v>5</v>
+      </c>
+      <c r="H20" s="35">
+        <v>6</v>
+      </c>
+      <c r="I20" s="35">
+        <v>7</v>
+      </c>
+      <c r="J20" s="35">
+        <v>8</v>
+      </c>
+      <c r="K20" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="31">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="C21" s="31">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="D21" s="31">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="E21" s="31">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="F21" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="G21" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="31">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="I21" s="31">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="J21" s="31">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K21" s="39">
+        <f>AVERAGE(B21:J21)</f>
+        <v>0.19044444444444442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="B22" s="32">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C22" s="32">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="D22" s="32">
+        <v>0.04</v>
+      </c>
+      <c r="E22" s="32">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F22" s="32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G22" s="32">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="H22" s="32">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I22" s="32">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J22" s="32">
+        <v>1.06E-2</v>
+      </c>
+      <c r="K22" s="39">
+        <f t="shared" ref="K22:K27" si="0">AVERAGE(B22:J22)</f>
+        <v>5.340000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="38">
+        <v>1E-3</v>
+      </c>
+      <c r="B23" s="29">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C23" s="29">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D23" s="34">
+        <v>0.03</v>
+      </c>
+      <c r="E23" s="34">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="F23" s="29">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G23" s="29">
+        <v>0.124</v>
+      </c>
+      <c r="H23" s="29">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I23" s="29">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J23" s="34">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="K23" s="39">
+        <f t="shared" si="0"/>
+        <v>3.6144444444444444E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="37">
+        <v>0.01</v>
+      </c>
+      <c r="B24" s="33">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C24" s="33">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D24" s="32">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E24" s="32">
+        <v>1E-3</v>
+      </c>
+      <c r="F24" s="33">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G24" s="32">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="H24" s="32">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I24" s="32">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J24" s="32">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="K24" s="39">
+        <f t="shared" si="0"/>
+        <v>2.3222222222222224E-2</v>
+      </c>
+      <c r="L24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="B25" s="29">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C25" s="29">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="D25" s="29">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E25" s="29">
+        <v>2E-3</v>
+      </c>
+      <c r="F25" s="29">
+        <v>0.03</v>
+      </c>
+      <c r="G25" s="29">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H25" s="34">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I25" s="34">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J25" s="29">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K25" s="39">
+        <f t="shared" si="0"/>
+        <v>2.5666666666666667E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="37">
+        <v>1</v>
+      </c>
+      <c r="B26" s="32">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="C26" s="32">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D26" s="32">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E26" s="32">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F26" s="32">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G26" s="33">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H26" s="32">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I26" s="32">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J26" s="32">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="K26" s="39">
+        <f t="shared" si="0"/>
+        <v>2.8777777777777777E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="38">
+        <v>10</v>
+      </c>
+      <c r="B27" s="29">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="C27" s="29">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D27" s="29">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="E27" s="29">
+        <v>0.03</v>
+      </c>
+      <c r="F27" s="29">
+        <v>6.3E-2</v>
+      </c>
+      <c r="G27" s="29">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H27" s="29">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I27" s="29">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="J27" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="K27" s="39">
+        <f t="shared" si="0"/>
+        <v>6.5555555555555561E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="37">
+        <v>100</v>
+      </c>
+      <c r="B28" s="32">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="C28" s="32">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="D28" s="32">
+        <v>0.311</v>
+      </c>
+      <c r="E28" s="32">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="F28" s="32">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="G28" s="32">
+        <v>0.12</v>
+      </c>
+      <c r="H28" s="32">
+        <v>0.372</v>
+      </c>
+      <c r="I28" s="32">
+        <v>0.316</v>
+      </c>
+      <c r="J28" s="33">
+        <v>0.432</v>
+      </c>
+      <c r="K28" s="39">
+        <f>AVERAGE(B28:J28)</f>
+        <v>0.28911111111111104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B29" s="39">
+        <f t="shared" ref="B29:I29" si="1">AVERAGE(B21:B28)</f>
+        <v>6.4375000000000002E-2</v>
+      </c>
+      <c r="C29" s="39">
+        <f t="shared" si="1"/>
+        <v>0.1195</v>
+      </c>
+      <c r="D29" s="39">
+        <f t="shared" si="1"/>
+        <v>8.0499999999999988E-2</v>
+      </c>
+      <c r="E29" s="39">
+        <f t="shared" si="1"/>
+        <v>5.0100000000000006E-2</v>
+      </c>
+      <c r="F29" s="39">
+        <f t="shared" si="1"/>
+        <v>8.7125000000000008E-2</v>
+      </c>
+      <c r="G29" s="39">
+        <f t="shared" si="1"/>
+        <v>7.3374999999999996E-2</v>
+      </c>
+      <c r="H29" s="39">
+        <f t="shared" si="1"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="I29" s="39">
+        <f t="shared" si="1"/>
+        <v>7.1124999999999994E-2</v>
+      </c>
+      <c r="J29" s="39">
+        <f>AVERAGE(J21:J28)</f>
+        <v>8.0262500000000001E-2</v>
+      </c>
+      <c r="K29" s="39"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="40">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>4</v>
+      </c>
+      <c r="G35" s="1">
+        <v>5</v>
+      </c>
+      <c r="H35" s="1">
+        <v>6</v>
+      </c>
+      <c r="I35" s="1">
+        <v>7</v>
+      </c>
+      <c r="J35" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="110.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="41">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="C36" s="26">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="D36" s="26">
+        <v>2.7799999999999998E-2</v>
+      </c>
+      <c r="E36" s="26">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="F36" s="42">
+        <v>2.6800000000000001E-2</v>
+      </c>
+      <c r="G36" s="42">
+        <v>2.3400000000000001E-2</v>
+      </c>
+      <c r="H36" s="26">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="I36" s="26">
+        <v>1.67E-2</v>
+      </c>
+      <c r="J36" s="42">
+        <v>1.7500000000000002E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>